<commit_message>
added price and buyer functionality
</commit_message>
<xml_diff>
--- a/output/DATA_BUKU.xlsx
+++ b/output/DATA_BUKU.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="181029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -394,7 +394,7 @@
   <dimension ref="A1:G419"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D421" sqref="D421"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
@@ -435,7 +435,7 @@
       </c>
       <c r="F1" s="3" t="inlineStr">
         <is>
-          <t>/</t>
+          <t>Tick?</t>
         </is>
       </c>
       <c r="G1" s="3" t="inlineStr">
@@ -507,9 +507,19 @@
       <c r="D4" s="2" t="n">
         <v>5</v>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>3.00</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>/</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>HAZIMI</t>
         </is>
       </c>
     </row>
@@ -1341,6 +1351,21 @@
       <c r="D48" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>3.</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>dasd</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1869,6 +1894,21 @@
       <c r="D76" s="2" t="inlineStr">
         <is>
           <t>FREE</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>8.03</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>HOLA</t>
         </is>
       </c>
     </row>

</xml_diff>